<commit_message>
Edit Last Meeting Updated
</commit_message>
<xml_diff>
--- a/src/assets/GSMs.xlsx
+++ b/src/assets/GSMs.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA1C53B-7A2E-43AC-98D7-DD661EE562B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4C879B-29F9-4574-B308-4F27C2D07967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{270DF063-4D78-4A52-8DA2-A7D9B87D9F57}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="GSMs" sheetId="1" r:id="rId1"/>
+    <sheet name="Values" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t>2G</t>
   </si>
@@ -190,6 +191,13 @@
   </si>
   <si>
     <t>Tartous</t>
+  </si>
+  <si>
+    <t>Initialize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: Red Columns are Required
+</t>
   </si>
 </sst>
 </file>
@@ -234,7 +242,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -257,17 +265,68 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,15 +641,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38E92CD3-B684-451F-A705-974C10A95FBE}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
@@ -601,25 +660,26 @@
     <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -641,23 +701,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -665,350 +715,605 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="N3" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="N5" s="8"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="N10" s="5"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="N3:N5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3CBCAB86-D042-45A2-B7CE-1BEBCBD0ED9E}">
+          <x14:formula1>
+            <xm:f>Values!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0F5537CE-EFBB-4181-865C-3C60286E5A5D}">
+          <x14:formula1>
+            <xm:f>Values!$B$2:$B$22</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6A84E8CF-9C38-4301-A5EE-6F89340732C8}">
+          <x14:formula1>
+            <xm:f>Values!$C$2:$C$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DA28CCE6-0E7F-44C2-8313-436F495ABF35}">
+          <x14:formula1>
+            <xm:f>Values!$D$2:$D$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7C811C4C-C565-4069-BD0B-3F972648ABB3}">
+          <x14:formula1>
+            <xm:f>Values!$E$2:$E$14</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84B0961B-323E-46CE-8D19-54C9F1C4CDE7}">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1" t="s">
-        <v>39</v>
-      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1" t="s">
-        <v>40</v>
-      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1" t="s">
-        <v>41</v>
-      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1" t="s">
-        <v>42</v>
-      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1" t="s">
-        <v>43</v>
-      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1" t="s">
-        <v>44</v>
-      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Edit general statistics view
</commit_message>
<xml_diff>
--- a/src/assets/GSMs.xlsx
+++ b/src/assets/GSMs.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Syriatel\NewTemplate\NewTemplate\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4C879B-29F9-4574-B308-4F27C2D07967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5647CEBE-D4A1-444E-9036-621A0F473066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{270DF063-4D78-4A52-8DA2-A7D9B87D9F57}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{270DF063-4D78-4A52-8DA2-A7D9B87D9F57}"/>
   </bookViews>
   <sheets>
     <sheet name="GSMs" sheetId="1" r:id="rId1"/>
     <sheet name="Values" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
   <si>
     <t>2G</t>
   </si>
@@ -194,10 +194,6 @@
   </si>
   <si>
     <t>Initialize</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Note: Red Columns are Required
-</t>
   </si>
 </sst>
 </file>
@@ -242,7 +238,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -265,68 +261,19 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38E92CD3-B684-451F-A705-974C10A95FBE}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,10 +607,9 @@
     <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -701,7 +647,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -715,296 +661,43 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="N3" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="N4" s="7"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="N5" s="8"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="N10" s="5"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="N3:N5"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -1062,7 +755,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">

</xml_diff>